<commit_message>
modificacion del formulario 11
</commit_message>
<xml_diff>
--- a/Anotaciones.xlsx
+++ b/Anotaciones.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\progrmas_presupuestales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\progrmas_presupuestales\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D02E799-F8E5-4014-9DA4-81D884429E67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="810" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="810" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato 1. Documentación de pol" sheetId="1" r:id="rId1"/>
@@ -30,23 +31,28 @@
     <sheet name="Formato 16. Costeo por componen" sheetId="16" r:id="rId16"/>
     <sheet name="Formato 17. Fuentes de financia" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Wilbert Suárez Solis</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -75,12 +81,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Wilbert Suárez Solis</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1548,7 +1554,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -2444,53 +2450,71 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2498,92 +2522,110 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2594,54 +2636,39 @@
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2651,26 +2678,17 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2686,18 +2704,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3258,7 +3264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -3414,7 +3420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -3432,134 +3438,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="114" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="114" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="115" t="s">
+      <c r="E1" s="114" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
     </row>
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="128" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="131" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="126" t="s">
+      <c r="D3" s="133" t="s">
         <v>225</v>
       </c>
-      <c r="E3" s="126"/>
+      <c r="E3" s="133"/>
     </row>
     <row r="4" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="131"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
     </row>
     <row r="5" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="132" t="s">
+      <c r="C5" s="129" t="s">
         <v>259</v>
       </c>
-      <c r="D5" s="128" t="s">
+      <c r="D5" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="E5" s="126" t="s">
+      <c r="E5" s="133" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="131"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="127"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="134"/>
     </row>
     <row r="7" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="126" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="129" t="s">
         <v>229</v>
       </c>
-      <c r="D7" s="128" t="s">
+      <c r="D7" s="131" t="s">
         <v>230</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="133" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="131"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="127"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="134"/>
     </row>
     <row r="9" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="66"/>
-      <c r="B9" s="134" t="s">
+      <c r="B9" s="126" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="129" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="128" t="s">
+      <c r="D9" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="E9" s="126" t="s">
+      <c r="E9" s="133" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="127"/>
+      <c r="B10" s="127"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="134"/>
     </row>
     <row r="11" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="66"/>
-      <c r="B11" s="134" t="s">
+      <c r="B11" s="126" t="s">
         <v>237</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="129" t="s">
         <v>238</v>
       </c>
-      <c r="D11" s="132" t="s">
+      <c r="D11" s="129" t="s">
         <v>239</v>
       </c>
-      <c r="E11" s="126" t="s">
+      <c r="E11" s="133" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="130"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="126"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="133"/>
     </row>
     <row r="13" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3706,17 +3712,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="B1:B2"/>
@@ -3730,6 +3725,17 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3737,11 +3743,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,136 +3760,136 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="135" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="145" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="136" t="s">
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="145" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="136"/>
-      <c r="B4" s="142"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="136"/>
+      <c r="A4" s="145"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="145"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="136"/>
-      <c r="B5" s="135" t="s">
+      <c r="A5" s="145"/>
+      <c r="B5" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="135" t="s">
+      <c r="C5" s="147" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="147" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="145" t="s">
+      <c r="E5" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
-      <c r="I5" s="146"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="136"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="144"/>
+      <c r="K5" s="145"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="136"/>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="144"/>
-      <c r="K6" s="136"/>
+      <c r="A6" s="145"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="139"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="145"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="135" t="s">
+      <c r="A7" s="145"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="147" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="135" t="s">
+      <c r="F7" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="135" t="s">
+      <c r="G7" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="135" t="s">
+      <c r="H7" s="147" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="135" t="s">
+      <c r="I7" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="135" t="s">
+      <c r="J7" s="147" t="s">
         <v>94</v>
       </c>
-      <c r="K7" s="136"/>
+      <c r="K7" s="145"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="136"/>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
+      <c r="A8" s="145"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="145"/>
+      <c r="K8" s="145"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="137"/>
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="137"/>
-      <c r="I9" s="137"/>
-      <c r="J9" s="137"/>
-      <c r="K9" s="137"/>
+      <c r="A9" s="146"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="146"/>
+      <c r="D9" s="146"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="146"/>
+      <c r="J9" s="146"/>
+      <c r="K9" s="146"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
@@ -3936,7 +3942,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="135" t="s">
+      <c r="A12" s="147" t="s">
         <v>96</v>
       </c>
       <c r="B12" s="119"/>
@@ -3951,17 +3957,17 @@
       <c r="K12" s="119"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="137"/>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
+      <c r="A13" s="146"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
     </row>
     <row r="14" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51" t="s">
@@ -4111,13 +4117,23 @@
       <c r="C19" s="64"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="113" t="s">
         <v>388</v>
       </c>
-      <c r="B21" s="101"/>
+      <c r="B21" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E7:E9"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:J4"/>
     <mergeCell ref="E5:J6"/>
@@ -4134,23 +4150,14 @@
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="K3:K9"/>
     <mergeCell ref="J7:J9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D5:D9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4168,22 +4175,22 @@
       <c r="A1" s="38"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="162" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="150"/>
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
+      <c r="A3" s="162"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
       <c r="E3" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="163" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="39" t="s">
@@ -4194,7 +4201,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="152"/>
+      <c r="A5" s="149"/>
       <c r="B5" s="26" t="s">
         <v>390</v>
       </c>
@@ -4206,34 +4213,34 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="154" t="s">
+      <c r="A6" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
+      <c r="B6" s="154"/>
+      <c r="C6" s="155"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="148" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="161" t="s">
+      <c r="B7" s="156" t="s">
         <v>391</v>
       </c>
-      <c r="C7" s="162"/>
+      <c r="C7" s="157"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="152"/>
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
+      <c r="A8" s="149"/>
+      <c r="B8" s="158"/>
+      <c r="C8" s="159"/>
     </row>
     <row r="9" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="148" t="s">
+      <c r="B9" s="160" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="149"/>
+      <c r="C9" s="161"/>
       <c r="E9" s="125" t="s">
         <v>371</v>
       </c>
@@ -4243,28 +4250,28 @@
       <c r="I9" s="125"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="159"/>
-      <c r="C10" s="160"/>
+      <c r="B10" s="151"/>
+      <c r="C10" s="152"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="148" t="s">
+      <c r="A11" s="160" t="s">
         <v>261</v>
       </c>
-      <c r="B11" s="157"/>
-      <c r="C11" s="149"/>
+      <c r="B11" s="164"/>
+      <c r="C11" s="161"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="154" t="s">
+      <c r="A12" s="153" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="155"/>
-      <c r="C12" s="156"/>
+      <c r="B12" s="154"/>
+      <c r="C12" s="155"/>
     </row>
     <row r="13" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="148" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -4275,7 +4282,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="152"/>
+      <c r="A14" s="149"/>
       <c r="B14" s="40" t="s">
         <v>107</v>
       </c>
@@ -4284,7 +4291,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="151" t="s">
+      <c r="A15" s="148" t="s">
         <v>108</v>
       </c>
       <c r="B15" s="40" t="s">
@@ -4295,7 +4302,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="152"/>
+      <c r="A16" s="149"/>
       <c r="B16" s="40" t="s">
         <v>107</v>
       </c>
@@ -4304,7 +4311,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="151" t="s">
+      <c r="A17" s="148" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="40" t="s">
@@ -4313,14 +4320,14 @@
       <c r="C17" s="26"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="152"/>
+      <c r="A18" s="149"/>
       <c r="B18" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="151" t="s">
+      <c r="A19" s="148" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="40" t="s">
@@ -4329,18 +4336,18 @@
       <c r="C19" s="26"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="152"/>
+      <c r="A20" s="149"/>
       <c r="B20" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C20" s="26"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="150" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="159"/>
-      <c r="C21" s="160"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="152"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="41" t="s">
@@ -4365,11 +4372,11 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="154" t="s">
+      <c r="A24" s="153" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="156"/>
+      <c r="B24" s="154"/>
+      <c r="C24" s="155"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
@@ -4394,65 +4401,59 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="154" t="s">
+      <c r="A27" s="153" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="156"/>
+      <c r="B27" s="154"/>
+      <c r="C27" s="155"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="148" t="s">
+      <c r="B28" s="160" t="s">
         <v>265</v>
       </c>
-      <c r="C28" s="149"/>
+      <c r="C28" s="161"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="148" t="s">
+      <c r="B29" s="160" t="s">
         <v>266</v>
       </c>
-      <c r="C29" s="149"/>
+      <c r="C29" s="161"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="160" t="s">
         <v>267</v>
       </c>
-      <c r="C30" s="149"/>
+      <c r="C30" s="161"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="148" t="s">
+      <c r="B31" s="160" t="s">
         <v>268</v>
       </c>
-      <c r="C31" s="149"/>
+      <c r="C31" s="161"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="148" t="s">
+      <c r="B32" s="160" t="s">
         <v>269</v>
       </c>
-      <c r="C32" s="149"/>
+      <c r="C32" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:C10"/>
     <mergeCell ref="E9:I9"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="A2:C3"/>
@@ -4469,13 +4470,19 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4503,34 +4510,34 @@
       <c r="B2" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="114" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="114" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="115" t="s">
+      <c r="E2" s="114" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="114" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="115" t="s">
+      <c r="G2" s="114" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="115" t="s">
+      <c r="H2" s="114" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="166"/>
       <c r="B3" s="48"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
     </row>
     <row r="4" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
@@ -4775,7 +4782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4816,8 +4823,8 @@
     </row>
     <row r="4" spans="1:3" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="99"/>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
@@ -4843,8 +4850,8 @@
     </row>
     <row r="7" spans="1:3" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="99"/>
-      <c r="B7" s="120"/>
-      <c r="C7" s="120"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="100" t="s">
@@ -4859,8 +4866,8 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="99"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -4890,7 +4897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4912,166 +4919,166 @@
       <c r="A1" s="33"/>
     </row>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="109" t="s">
         <v>133</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="175" t="s">
+      <c r="C2" s="167" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="175" t="s">
+      <c r="E2" s="167" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="104" t="s">
+      <c r="F2" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="175" t="s">
+      <c r="G2" s="167" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="104" t="s">
+      <c r="H2" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="175" t="s">
+      <c r="I2" s="167" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="167" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="104" t="s">
+      <c r="L2" s="109" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="105"/>
+      <c r="A3" s="104"/>
       <c r="B3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="104"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="167"/>
+      <c r="L3" s="109"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="167" t="s">
+      <c r="A4" s="174" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="172">
+      <c r="B4" s="169">
         <f>C4+E4+G4+I4+K4</f>
         <v>60019</v>
       </c>
-      <c r="C4" s="172">
+      <c r="C4" s="169">
         <f>C6+C8</f>
         <v>11973</v>
       </c>
-      <c r="D4" s="173">
+      <c r="D4" s="170">
         <f>C4/$N$5</f>
         <v>0.56513735485698102</v>
       </c>
-      <c r="E4" s="172">
+      <c r="E4" s="169">
         <f>E6+E8</f>
         <v>11872</v>
       </c>
-      <c r="F4" s="173">
+      <c r="F4" s="170">
         <f>E4/$N$5</f>
         <v>0.56037005569715848</v>
       </c>
-      <c r="G4" s="172">
+      <c r="G4" s="169">
         <f>G6+G8</f>
         <v>12090</v>
       </c>
-      <c r="H4" s="173">
+      <c r="H4" s="170">
         <f>G4/$N$5</f>
         <v>0.57065986972529026</v>
       </c>
-      <c r="I4" s="172">
+      <c r="I4" s="169">
         <f>I6+I8</f>
         <v>11732</v>
       </c>
-      <c r="J4" s="173">
+      <c r="J4" s="170">
         <f>I4/$N$5</f>
         <v>0.55376191824789955</v>
       </c>
-      <c r="K4" s="172">
+      <c r="K4" s="169">
         <f>K6+K8</f>
         <v>12352</v>
       </c>
-      <c r="L4" s="173">
+      <c r="L4" s="170">
         <f>K4/$N$5</f>
         <v>0.5830265269517606</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="168"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="174"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="174"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="174"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="174"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="174"/>
+      <c r="A5" s="175"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="171"/>
       <c r="N5">
         <f>N6+N7</f>
         <v>21186</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="167" t="s">
+      <c r="A6" s="174" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="172">
+      <c r="B6" s="169">
         <f>C6+E6+G6+I6+K6</f>
         <v>26772</v>
       </c>
-      <c r="C6" s="172">
+      <c r="C6" s="169">
         <v>5153</v>
       </c>
-      <c r="D6" s="173">
+      <c r="D6" s="170">
         <f>C6/$N$6</f>
         <v>0.41506242448650826</v>
       </c>
-      <c r="E6" s="172">
+      <c r="E6" s="169">
         <v>5422</v>
       </c>
-      <c r="F6" s="173">
+      <c r="F6" s="170">
         <f>E6/$N$6</f>
         <v>0.43672976238421263</v>
       </c>
-      <c r="G6" s="172">
+      <c r="G6" s="169">
         <v>4890</v>
       </c>
-      <c r="H6" s="173">
+      <c r="H6" s="170">
         <f>G6/$N$6</f>
         <v>0.39387837293596456</v>
       </c>
-      <c r="I6" s="172">
+      <c r="I6" s="169">
         <v>5133</v>
       </c>
-      <c r="J6" s="173">
+      <c r="J6" s="170">
         <f>I6/$N$6</f>
         <v>0.4134514699959726</v>
       </c>
-      <c r="K6" s="172">
+      <c r="K6" s="169">
         <v>6174</v>
       </c>
-      <c r="L6" s="173">
+      <c r="L6" s="170">
         <f>K6/$N$6</f>
         <v>0.49730165122835279</v>
       </c>
@@ -5080,86 +5087,86 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="168"/>
-      <c r="B7" s="120"/>
-      <c r="C7" s="120"/>
-      <c r="D7" s="174"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="174"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="174"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="174"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="174"/>
+      <c r="A7" s="175"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="171"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="171"/>
       <c r="N7">
         <v>8771</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="167" t="s">
+      <c r="A8" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="172">
+      <c r="B8" s="169">
         <f>C8+E8+G8+I8+K8</f>
         <v>33247</v>
       </c>
-      <c r="C8" s="172">
+      <c r="C8" s="169">
         <v>6820</v>
       </c>
-      <c r="D8" s="173">
+      <c r="D8" s="170">
         <f>C8/$N$7</f>
         <v>0.77756242161669142</v>
       </c>
-      <c r="E8" s="172">
+      <c r="E8" s="169">
         <v>6450</v>
       </c>
-      <c r="F8" s="173">
+      <c r="F8" s="170">
         <f>E8/$N$7</f>
         <v>0.73537795006270668</v>
       </c>
-      <c r="G8" s="172">
+      <c r="G8" s="169">
         <v>7200</v>
       </c>
-      <c r="H8" s="173">
+      <c r="H8" s="170">
         <f>G8/$N$7</f>
         <v>0.82088701402348652</v>
       </c>
-      <c r="I8" s="172">
+      <c r="I8" s="169">
         <v>6599</v>
       </c>
-      <c r="J8" s="173">
+      <c r="J8" s="170">
         <f>I8/$N$7</f>
         <v>0.75236575076958156</v>
       </c>
-      <c r="K8" s="172">
+      <c r="K8" s="169">
         <v>6178</v>
       </c>
-      <c r="L8" s="173">
+      <c r="L8" s="170">
         <f>K8/$N$7</f>
         <v>0.70436666286626382</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="168"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="174"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="174"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="174"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="174"/>
+      <c r="A9" s="175"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="171"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="171"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="171"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="167" t="s">
+      <c r="A10" s="174" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="119"/>
-      <c r="C10" s="172">
+      <c r="C10" s="169">
         <v>1092</v>
       </c>
       <c r="D10" s="119"/>
@@ -5173,24 +5180,24 @@
       <c r="L10" s="119"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="168"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
+      <c r="A11" s="175"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="167" t="s">
+      <c r="A12" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="170" t="s">
+      <c r="B12" s="172" t="s">
         <v>392</v>
       </c>
       <c r="C12" s="119"/>
@@ -5205,24 +5212,24 @@
       <c r="L12" s="119"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="168"/>
-      <c r="B13" s="171"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
+      <c r="A13" s="175"/>
+      <c r="B13" s="173"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="118"/>
     </row>
     <row r="14" spans="1:14" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="167" t="s">
+      <c r="A14" s="174" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="170" t="s">
+      <c r="B14" s="172" t="s">
         <v>163</v>
       </c>
       <c r="C14" s="119"/>
@@ -5237,32 +5244,32 @@
       <c r="L14" s="119"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="168"/>
-      <c r="B15" s="171"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
+      <c r="A15" s="175"/>
+      <c r="B15" s="173"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="169" t="s">
+      <c r="A16" s="176" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="169"/>
-      <c r="C16" s="169"/>
-      <c r="D16" s="169"/>
+      <c r="B16" s="176"/>
+      <c r="C16" s="176"/>
+      <c r="D16" s="176"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="169" t="s">
+      <c r="A17" s="176" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="169"/>
+      <c r="B17" s="176"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
     </row>
@@ -5283,70 +5290,11 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
@@ -5363,11 +5311,70 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5375,7 +5382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -5400,56 +5407,56 @@
       <c r="A1" s="11"/>
     </row>
     <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="184" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="162" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="177" t="s">
+      <c r="C2" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="184" t="s">
+      <c r="E2" s="177" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="184" t="s">
+      <c r="G2" s="177" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="182" t="s">
+      <c r="H2" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="184" t="s">
+      <c r="I2" s="177" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="182" t="s">
+      <c r="J2" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="184" t="s">
+      <c r="K2" s="177" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="182" t="s">
+      <c r="L2" s="179" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="181"/>
-      <c r="B3" s="179"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="183"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="183"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="183"/>
+      <c r="A3" s="185"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="180"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="178"/>
+      <c r="J3" s="180"/>
+      <c r="K3" s="178"/>
+      <c r="L3" s="180"/>
     </row>
     <row r="4" spans="1:14" ht="25.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
@@ -6118,6 +6125,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="H2:H3"/>
@@ -6125,18 +6137,13 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6285,7 +6292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6390,7 +6397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6584,7 +6591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6719,11 +6726,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6801,19 +6808,19 @@
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="103" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="112" t="s">
+      <c r="E6" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="112" t="s">
+      <c r="F6" s="103" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6821,13 +6828,13 @@
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="105"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
@@ -6844,26 +6851,26 @@
       <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="106" t="s">
+      <c r="C9" s="105" t="s">
         <v>381</v>
       </c>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
+      <c r="A10" s="111"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="106"/>
     </row>
     <row r="11" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -6900,56 +6907,56 @@
       <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="106" t="s">
+      <c r="C13" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="110"/>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
+      <c r="A14" s="111"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="106"/>
       <c r="D14" s="107"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="109" t="s">
         <v>183</v>
       </c>
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="109" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="104" t="s">
+      <c r="E15" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="104" t="s">
+      <c r="F15" s="109" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="105"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="105"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
     </row>
     <row r="17" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
@@ -6974,23 +6981,23 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="108" t="s">
+      <c r="A18" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="C18" s="106" t="s">
+      <c r="C18" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="D18" s="106" t="s">
+      <c r="D18" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109"/>
+      <c r="A19" s="112"/>
       <c r="B19" s="107"/>
       <c r="C19" s="107"/>
       <c r="D19" s="107"/>
@@ -6998,34 +7005,34 @@
       <c r="F19" s="107"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="104" t="s">
+      <c r="A20" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="102" t="s">
+      <c r="B20" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="104" t="s">
+      <c r="C20" s="109" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="104" t="s">
+      <c r="E20" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="104" t="s">
+      <c r="F20" s="109" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="105"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="104"/>
       <c r="D21" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
     </row>
     <row r="22" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -7042,21 +7049,21 @@
       <c r="F22" s="55"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="106" t="s">
+      <c r="C23" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="D23" s="106"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="109"/>
+      <c r="A24" s="112"/>
       <c r="B24" s="107"/>
       <c r="C24" s="107"/>
       <c r="D24" s="107"/>
@@ -7064,10 +7071,10 @@
       <c r="F24" s="107"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="101" t="s">
+      <c r="B26" s="113" t="s">
         <v>351</v>
       </c>
-      <c r="C26" s="101"/>
+      <c r="C26" s="113"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -7082,6 +7089,31 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="E6:E7"/>
@@ -7096,31 +7128,6 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7128,7 +7135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -7155,67 +7162,67 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="114" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="115" t="s">
+      <c r="E2" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
     </row>
     <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115"/>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115" t="s">
+      <c r="A3" s="114"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" s="114" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="115" t="s">
+      <c r="J3" s="114" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="115" t="s">
+      <c r="K3" s="114" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="116"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
+      <c r="A4" s="115"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
@@ -7367,10 +7374,10 @@
       <c r="B13" t="s">
         <v>304</v>
       </c>
-      <c r="C13" s="114" t="s">
+      <c r="C13" s="116" t="s">
         <v>355</v>
       </c>
-      <c r="D13" s="114"/>
+      <c r="D13" s="116"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
@@ -7379,6 +7386,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:K2"/>
@@ -7387,18 +7399,13 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7432,17 +7439,17 @@
       <c r="A4" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="120" t="s">
         <v>356</v>
       </c>
-      <c r="C4" s="122" t="s">
+      <c r="C4" s="120" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="99"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="100" t="s">
@@ -7456,25 +7463,25 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="118"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
+      <c r="A7" s="124"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="123" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="124" t="s">
+      <c r="B8" s="122" t="s">
         <v>358</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="122" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="99"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="100" t="s">
@@ -7489,8 +7496,8 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="118"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="100" t="s">
@@ -7505,22 +7512,22 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="99"/>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="117" t="s">
         <v>360</v>
       </c>
       <c r="C14" s="119"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="99"/>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="118"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -7532,6 +7539,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B4:B5"/>
@@ -7540,26 +7557,16 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -7733,7 +7740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7757,28 +7764,28 @@
       <c r="A2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="114" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="115"/>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
+      <c r="A4" s="114"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
     </row>
     <row r="5" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">

</xml_diff>

<commit_message>
Se realizan anotaciones al archivo
</commit_message>
<xml_diff>
--- a/Anotaciones.xlsx
+++ b/Anotaciones.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\progrmas_presupuestales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\progrmas_presupuestales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="810" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="810" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Formato 1. Documentación de pol" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,10 @@
     <sheet name="Formato 16. Costeo por componen" sheetId="16" r:id="rId16"/>
     <sheet name="Formato 17. Fuentes de financia" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Formato 5. Identificación y cua'!$A$1:$F$26</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="398">
   <si>
     <t>Política o programa</t>
   </si>
@@ -1441,15 +1443,6 @@
     <t>¿todas las columnas son de text abierto?</t>
   </si>
   <si>
-    <t>¿ es catalogo?</t>
-  </si>
-  <si>
-    <t>¿ estas areas se capturan cuando se da de alta la dependencia, en todo caso seria un combo?</t>
-  </si>
-  <si>
-    <t>¿ las dependencias tienen relaciones o simplemente es un catalogo?</t>
-  </si>
-  <si>
     <t>¿esta columna se hace de forma manual?</t>
   </si>
   <si>
@@ -1515,15 +1508,9 @@
     <t>en esta columna son los mismo bienes y servicios del formato 3? Combo</t>
   </si>
   <si>
-    <t>¿ estas son las instituciones relacionadas? Combo</t>
-  </si>
-  <si>
     <t>Subsecretaría del Trabajo combo</t>
   </si>
   <si>
-    <t xml:space="preserve">comob </t>
-  </si>
-  <si>
     <t>TODO ESTE FORMATO PENDIENTE</t>
   </si>
   <si>
@@ -1543,12 +1530,39 @@
   </si>
   <si>
     <t>campo abierto con un boton guardar, manejar los mismos elementos</t>
+  </si>
+  <si>
+    <t>Va a ser texto</t>
+  </si>
+  <si>
+    <t>PURO TEXTO</t>
+  </si>
+  <si>
+    <t>CATALOGO (UNIDAD DE MEDIDA)</t>
+  </si>
+  <si>
+    <t>COMBO</t>
+  </si>
+  <si>
+    <t>TEXTO</t>
+  </si>
+  <si>
+    <t>texto</t>
+  </si>
+  <si>
+    <t>FORMATO  1</t>
+  </si>
+  <si>
+    <t>Formato 2</t>
+  </si>
+  <si>
+    <t>Formato 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -2160,7 +2174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2417,6 +2431,12 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2444,53 +2464,71 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2498,92 +2536,110 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2594,54 +2650,39 @@
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2651,26 +2692,17 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2686,18 +2718,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2737,7 +2757,7 @@
         <xdr:cNvPr id="8195" name="Text Box 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B088419-5395-49DB-ABCE-DCF627D04AAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B088419-5395-49DB-ABCE-DCF627D04AAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2817,7 +2837,7 @@
         <xdr:cNvPr id="8193" name="Text Box 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D505990-4389-48C5-81AE-2F28CAA46543}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D505990-4389-48C5-81AE-2F28CAA46543}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2897,7 +2917,7 @@
         <xdr:cNvPr id="8194" name="Text Box 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C4E20D9-3B0C-4E62-AC7D-D15BDAA741BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C4E20D9-3B0C-4E62-AC7D-D15BDAA741BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3259,10 +3279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,7 +3295,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3371,7 +3393,7 @@
     </row>
     <row r="6" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3380,36 +3402,9 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="46.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="56" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3417,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,24 +3427,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="116" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="116" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="115" t="s">
+      <c r="E1" s="116" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
     </row>
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3458,108 +3453,108 @@
       <c r="B3" s="130" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="133" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="126" t="s">
+      <c r="D3" s="135" t="s">
         <v>225</v>
       </c>
-      <c r="E3" s="126"/>
+      <c r="E3" s="135"/>
     </row>
     <row r="4" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="131"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
     </row>
     <row r="5" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="128" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="132" t="s">
+      <c r="C5" s="131" t="s">
         <v>259</v>
       </c>
-      <c r="D5" s="128" t="s">
+      <c r="D5" s="133" t="s">
         <v>227</v>
       </c>
-      <c r="E5" s="126" t="s">
+      <c r="E5" s="135" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="131"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="127"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="136"/>
     </row>
     <row r="7" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="128" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="131" t="s">
         <v>229</v>
       </c>
-      <c r="D7" s="128" t="s">
+      <c r="D7" s="133" t="s">
         <v>230</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="135" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="131"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="127"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="136"/>
     </row>
     <row r="9" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="66"/>
-      <c r="B9" s="134" t="s">
+      <c r="B9" s="128" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="131" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="128" t="s">
+      <c r="D9" s="133" t="s">
         <v>236</v>
       </c>
-      <c r="E9" s="126" t="s">
+      <c r="E9" s="135" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="127"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="134"/>
+      <c r="E10" s="136"/>
     </row>
     <row r="11" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="66"/>
-      <c r="B11" s="134" t="s">
+      <c r="B11" s="128" t="s">
         <v>237</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="131" t="s">
         <v>238</v>
       </c>
-      <c r="D11" s="132" t="s">
+      <c r="D11" s="131" t="s">
         <v>239</v>
       </c>
-      <c r="E11" s="126" t="s">
+      <c r="E11" s="135" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="130"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="126"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="135"/>
     </row>
     <row r="13" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3674,7 +3669,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="91" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
@@ -3682,16 +3677,16 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="86" t="s">
+        <v>363</v>
+      </c>
+      <c r="C23" s="88" t="s">
+        <v>364</v>
+      </c>
+      <c r="D23" s="87" t="s">
+        <v>365</v>
+      </c>
+      <c r="E23" s="89" t="s">
         <v>366</v>
-      </c>
-      <c r="C23" s="88" t="s">
-        <v>367</v>
-      </c>
-      <c r="D23" s="87" t="s">
-        <v>368</v>
-      </c>
-      <c r="E23" s="89" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -3701,22 +3696,11 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="86" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="B1:B2"/>
@@ -3730,6 +3714,17 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3740,8 +3735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,136 +3749,136 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="137" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="138" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="136" t="s">
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="147" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="136"/>
-      <c r="B4" s="142"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="136"/>
+      <c r="A4" s="147"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="147"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="136"/>
-      <c r="B5" s="135" t="s">
+      <c r="A5" s="147"/>
+      <c r="B5" s="149" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="135" t="s">
+      <c r="C5" s="149" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="149" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="145" t="s">
+      <c r="E5" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
-      <c r="I5" s="146"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="136"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="147"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="136"/>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="144"/>
-      <c r="K6" s="136"/>
+      <c r="A6" s="147"/>
+      <c r="B6" s="147"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
+      <c r="I6" s="142"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="147"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="135" t="s">
+      <c r="A7" s="147"/>
+      <c r="B7" s="147"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="149" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="135" t="s">
+      <c r="F7" s="149" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="135" t="s">
+      <c r="G7" s="149" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="135" t="s">
+      <c r="H7" s="149" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="135" t="s">
+      <c r="I7" s="149" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="135" t="s">
+      <c r="J7" s="149" t="s">
         <v>94</v>
       </c>
-      <c r="K7" s="136"/>
+      <c r="K7" s="147"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="136"/>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
+      <c r="A8" s="147"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="147"/>
+      <c r="K8" s="147"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="137"/>
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="137"/>
-      <c r="I9" s="137"/>
-      <c r="J9" s="137"/>
-      <c r="K9" s="137"/>
+      <c r="A9" s="148"/>
+      <c r="B9" s="148"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="148"/>
+      <c r="J9" s="148"/>
+      <c r="K9" s="148"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
@@ -3936,22 +3931,22 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="135" t="s">
+      <c r="A12" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="119"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="137"/>
+      <c r="A13" s="148"/>
       <c r="B13" s="120"/>
       <c r="C13" s="120"/>
       <c r="D13" s="120"/>
@@ -4105,19 +4100,29 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="89" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B19" s="64"/>
       <c r="C19" s="64"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="101" t="s">
-        <v>388</v>
-      </c>
-      <c r="B21" s="101"/>
+      <c r="A21" s="115" t="s">
+        <v>383</v>
+      </c>
+      <c r="B21" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E7:E9"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:J4"/>
     <mergeCell ref="E5:J6"/>
@@ -4134,16 +4139,6 @@
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="K3:K9"/>
     <mergeCell ref="J7:J9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D5:D9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4154,7 +4149,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4168,22 +4163,22 @@
       <c r="A1" s="38"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="150"/>
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
+      <c r="A3" s="164"/>
+      <c r="B3" s="164"/>
+      <c r="C3" s="164"/>
       <c r="E3" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="165" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="39" t="s">
@@ -4194,77 +4189,77 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="152"/>
+      <c r="A5" s="151"/>
       <c r="B5" s="26" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E5" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="154" t="s">
+      <c r="A6" s="155" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="157"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="150" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="161" t="s">
-        <v>391</v>
-      </c>
-      <c r="C7" s="162"/>
+      <c r="B7" s="158" t="s">
+        <v>386</v>
+      </c>
+      <c r="C7" s="159"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="152"/>
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
     </row>
     <row r="9" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="148" t="s">
+      <c r="B9" s="162" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="149"/>
-      <c r="E9" s="125" t="s">
-        <v>371</v>
-      </c>
-      <c r="F9" s="125"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="125"/>
+      <c r="C9" s="163"/>
+      <c r="E9" s="127" t="s">
+        <v>368</v>
+      </c>
+      <c r="F9" s="127"/>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="127"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="159"/>
-      <c r="C10" s="160"/>
+      <c r="B10" s="153"/>
+      <c r="C10" s="154"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="148" t="s">
+      <c r="A11" s="162" t="s">
         <v>261</v>
       </c>
-      <c r="B11" s="157"/>
-      <c r="C11" s="149"/>
+      <c r="B11" s="166"/>
+      <c r="C11" s="163"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="154" t="s">
+      <c r="A12" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="155"/>
-      <c r="C12" s="156"/>
+      <c r="B12" s="156"/>
+      <c r="C12" s="157"/>
     </row>
     <row r="13" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="150" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -4275,7 +4270,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="152"/>
+      <c r="A14" s="151"/>
       <c r="B14" s="40" t="s">
         <v>107</v>
       </c>
@@ -4284,7 +4279,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="151" t="s">
+      <c r="A15" s="150" t="s">
         <v>108</v>
       </c>
       <c r="B15" s="40" t="s">
@@ -4295,7 +4290,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="152"/>
+      <c r="A16" s="151"/>
       <c r="B16" s="40" t="s">
         <v>107</v>
       </c>
@@ -4304,7 +4299,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="151" t="s">
+      <c r="A17" s="150" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="40" t="s">
@@ -4313,14 +4308,14 @@
       <c r="C17" s="26"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="152"/>
+      <c r="A18" s="151"/>
       <c r="B18" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="151" t="s">
+      <c r="A19" s="150" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="40" t="s">
@@ -4329,18 +4324,18 @@
       <c r="C19" s="26"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="152"/>
+      <c r="A20" s="151"/>
       <c r="B20" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C20" s="26"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="159"/>
-      <c r="C21" s="160"/>
+      <c r="B21" s="153"/>
+      <c r="C21" s="154"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="41" t="s">
@@ -4365,11 +4360,11 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="154" t="s">
+      <c r="A24" s="155" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="156"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="157"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
@@ -4394,65 +4389,59 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="154" t="s">
+      <c r="A27" s="155" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="156"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="157"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="148" t="s">
+      <c r="B28" s="162" t="s">
         <v>265</v>
       </c>
-      <c r="C28" s="149"/>
+      <c r="C28" s="163"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="148" t="s">
+      <c r="B29" s="162" t="s">
         <v>266</v>
       </c>
-      <c r="C29" s="149"/>
+      <c r="C29" s="163"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="162" t="s">
         <v>267</v>
       </c>
-      <c r="C30" s="149"/>
+      <c r="C30" s="163"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="148" t="s">
+      <c r="B31" s="162" t="s">
         <v>268</v>
       </c>
-      <c r="C31" s="149"/>
+      <c r="C31" s="163"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="148" t="s">
+      <c r="B32" s="162" t="s">
         <v>269</v>
       </c>
-      <c r="C32" s="149"/>
+      <c r="C32" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:C10"/>
     <mergeCell ref="E9:I9"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="A2:C3"/>
@@ -4469,6 +4458,12 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4479,7 +4474,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4497,40 +4492,40 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="167" t="s">
         <v>166</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="116" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="116" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="115" t="s">
+      <c r="E2" s="116" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="116" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="115" t="s">
+      <c r="G2" s="116" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="115" t="s">
+      <c r="H2" s="116" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="166"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="48"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
     </row>
     <row r="4" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
@@ -4742,7 +4737,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="88" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C14" s="76" t="s">
         <v>322</v>
@@ -4776,10 +4771,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4804,18 +4799,18 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="102" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="121" t="s">
         <v>266</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="121" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="99"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="120"/>
       <c r="C4" s="120"/>
     </row>
@@ -4831,46 +4826,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="121" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="121" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="99"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="120"/>
       <c r="C7" s="120"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="100" t="s">
+      <c r="A8" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="121" t="s">
         <v>286</v>
       </c>
-      <c r="C8" s="119" t="s">
+      <c r="C8" s="121" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
+      <c r="A9" s="101"/>
       <c r="B9" s="120"/>
       <c r="C9" s="120"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>326</v>
+        <v>394</v>
       </c>
       <c r="B12" t="s">
         <v>306</v>
       </c>
       <c r="C12" t="s">
         <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4894,7 +4894,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E13"/>
+      <selection activeCell="J14" sqref="J14:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4912,166 +4912,166 @@
       <c r="A1" s="33"/>
     </row>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="111" t="s">
         <v>133</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="175" t="s">
+      <c r="C2" s="169" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="111" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="175" t="s">
+      <c r="E2" s="169" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="104" t="s">
+      <c r="F2" s="111" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="175" t="s">
+      <c r="G2" s="169" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="104" t="s">
+      <c r="H2" s="111" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="175" t="s">
+      <c r="I2" s="169" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="111" t="s">
         <v>137</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="169" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="104" t="s">
+      <c r="L2" s="111" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="105"/>
+      <c r="A3" s="106"/>
       <c r="B3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="104"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="111"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="167" t="s">
+      <c r="A4" s="176" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="172">
+      <c r="B4" s="171">
         <f>C4+E4+G4+I4+K4</f>
         <v>60019</v>
       </c>
-      <c r="C4" s="172">
+      <c r="C4" s="171">
         <f>C6+C8</f>
         <v>11973</v>
       </c>
-      <c r="D4" s="173">
+      <c r="D4" s="172">
         <f>C4/$N$5</f>
         <v>0.56513735485698102</v>
       </c>
-      <c r="E4" s="172">
+      <c r="E4" s="171">
         <f>E6+E8</f>
         <v>11872</v>
       </c>
-      <c r="F4" s="173">
+      <c r="F4" s="172">
         <f>E4/$N$5</f>
         <v>0.56037005569715848</v>
       </c>
-      <c r="G4" s="172">
+      <c r="G4" s="171">
         <f>G6+G8</f>
         <v>12090</v>
       </c>
-      <c r="H4" s="173">
+      <c r="H4" s="172">
         <f>G4/$N$5</f>
         <v>0.57065986972529026</v>
       </c>
-      <c r="I4" s="172">
+      <c r="I4" s="171">
         <f>I6+I8</f>
         <v>11732</v>
       </c>
-      <c r="J4" s="173">
+      <c r="J4" s="172">
         <f>I4/$N$5</f>
         <v>0.55376191824789955</v>
       </c>
-      <c r="K4" s="172">
+      <c r="K4" s="171">
         <f>K6+K8</f>
         <v>12352</v>
       </c>
-      <c r="L4" s="173">
+      <c r="L4" s="172">
         <f>K4/$N$5</f>
         <v>0.5830265269517606</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="168"/>
+      <c r="A5" s="177"/>
       <c r="B5" s="120"/>
       <c r="C5" s="120"/>
-      <c r="D5" s="174"/>
+      <c r="D5" s="173"/>
       <c r="E5" s="120"/>
-      <c r="F5" s="174"/>
+      <c r="F5" s="173"/>
       <c r="G5" s="120"/>
-      <c r="H5" s="174"/>
+      <c r="H5" s="173"/>
       <c r="I5" s="120"/>
-      <c r="J5" s="174"/>
+      <c r="J5" s="173"/>
       <c r="K5" s="120"/>
-      <c r="L5" s="174"/>
+      <c r="L5" s="173"/>
       <c r="N5">
         <f>N6+N7</f>
         <v>21186</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="167" t="s">
+      <c r="A6" s="176" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="172">
+      <c r="B6" s="171">
         <f>C6+E6+G6+I6+K6</f>
         <v>26772</v>
       </c>
-      <c r="C6" s="172">
+      <c r="C6" s="171">
         <v>5153</v>
       </c>
-      <c r="D6" s="173">
+      <c r="D6" s="172">
         <f>C6/$N$6</f>
         <v>0.41506242448650826</v>
       </c>
-      <c r="E6" s="172">
+      <c r="E6" s="171">
         <v>5422</v>
       </c>
-      <c r="F6" s="173">
+      <c r="F6" s="172">
         <f>E6/$N$6</f>
         <v>0.43672976238421263</v>
       </c>
-      <c r="G6" s="172">
+      <c r="G6" s="171">
         <v>4890</v>
       </c>
-      <c r="H6" s="173">
+      <c r="H6" s="172">
         <f>G6/$N$6</f>
         <v>0.39387837293596456</v>
       </c>
-      <c r="I6" s="172">
+      <c r="I6" s="171">
         <v>5133</v>
       </c>
-      <c r="J6" s="173">
+      <c r="J6" s="172">
         <f>I6/$N$6</f>
         <v>0.4134514699959726</v>
       </c>
-      <c r="K6" s="172">
+      <c r="K6" s="171">
         <v>6174</v>
       </c>
-      <c r="L6" s="173">
+      <c r="L6" s="172">
         <f>K6/$N$6</f>
         <v>0.49730165122835279</v>
       </c>
@@ -5080,100 +5080,100 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="168"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="120"/>
       <c r="C7" s="120"/>
-      <c r="D7" s="174"/>
+      <c r="D7" s="173"/>
       <c r="E7" s="120"/>
-      <c r="F7" s="174"/>
+      <c r="F7" s="173"/>
       <c r="G7" s="120"/>
-      <c r="H7" s="174"/>
+      <c r="H7" s="173"/>
       <c r="I7" s="120"/>
-      <c r="J7" s="174"/>
+      <c r="J7" s="173"/>
       <c r="K7" s="120"/>
-      <c r="L7" s="174"/>
+      <c r="L7" s="173"/>
       <c r="N7">
         <v>8771</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="167" t="s">
+      <c r="A8" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="172">
+      <c r="B8" s="171">
         <f>C8+E8+G8+I8+K8</f>
         <v>33247</v>
       </c>
-      <c r="C8" s="172">
+      <c r="C8" s="171">
         <v>6820</v>
       </c>
-      <c r="D8" s="173">
+      <c r="D8" s="172">
         <f>C8/$N$7</f>
         <v>0.77756242161669142</v>
       </c>
-      <c r="E8" s="172">
+      <c r="E8" s="171">
         <v>6450</v>
       </c>
-      <c r="F8" s="173">
+      <c r="F8" s="172">
         <f>E8/$N$7</f>
         <v>0.73537795006270668</v>
       </c>
-      <c r="G8" s="172">
+      <c r="G8" s="171">
         <v>7200</v>
       </c>
-      <c r="H8" s="173">
+      <c r="H8" s="172">
         <f>G8/$N$7</f>
         <v>0.82088701402348652</v>
       </c>
-      <c r="I8" s="172">
+      <c r="I8" s="171">
         <v>6599</v>
       </c>
-      <c r="J8" s="173">
+      <c r="J8" s="172">
         <f>I8/$N$7</f>
         <v>0.75236575076958156</v>
       </c>
-      <c r="K8" s="172">
+      <c r="K8" s="171">
         <v>6178</v>
       </c>
-      <c r="L8" s="173">
+      <c r="L8" s="172">
         <f>K8/$N$7</f>
         <v>0.70436666286626382</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="168"/>
+      <c r="A9" s="177"/>
       <c r="B9" s="120"/>
       <c r="C9" s="120"/>
-      <c r="D9" s="174"/>
+      <c r="D9" s="173"/>
       <c r="E9" s="120"/>
-      <c r="F9" s="174"/>
+      <c r="F9" s="173"/>
       <c r="G9" s="120"/>
-      <c r="H9" s="174"/>
+      <c r="H9" s="173"/>
       <c r="I9" s="120"/>
-      <c r="J9" s="174"/>
+      <c r="J9" s="173"/>
       <c r="K9" s="120"/>
-      <c r="L9" s="174"/>
+      <c r="L9" s="173"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="167" t="s">
+      <c r="A10" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="172">
+      <c r="B10" s="121"/>
+      <c r="C10" s="171">
         <v>1092</v>
       </c>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="168"/>
+      <c r="A11" s="177"/>
       <c r="B11" s="120"/>
       <c r="C11" s="120"/>
       <c r="D11" s="120"/>
@@ -5187,26 +5187,26 @@
       <c r="L11" s="120"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="167" t="s">
+      <c r="A12" s="176" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="170" t="s">
-        <v>392</v>
-      </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
+      <c r="B12" s="174" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="121"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="168"/>
-      <c r="B13" s="171"/>
+      <c r="A13" s="177"/>
+      <c r="B13" s="175"/>
       <c r="C13" s="120"/>
       <c r="D13" s="120"/>
       <c r="E13" s="120"/>
@@ -5219,26 +5219,26 @@
       <c r="L13" s="120"/>
     </row>
     <row r="14" spans="1:14" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="167" t="s">
+      <c r="A14" s="176" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="170" t="s">
+      <c r="B14" s="174" t="s">
         <v>163</v>
       </c>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="119"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="121"/>
+      <c r="L14" s="121"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="168"/>
-      <c r="B15" s="171"/>
+      <c r="A15" s="177"/>
+      <c r="B15" s="175"/>
       <c r="C15" s="120"/>
       <c r="D15" s="120"/>
       <c r="E15" s="120"/>
@@ -5251,24 +5251,24 @@
       <c r="L15" s="120"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="169" t="s">
+      <c r="A16" s="178" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="169"/>
-      <c r="C16" s="169"/>
-      <c r="D16" s="169"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="169" t="s">
+      <c r="A17" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="169"/>
+      <c r="B17" s="178"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -5283,70 +5283,11 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
@@ -5363,11 +5304,70 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5378,8 +5378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5400,56 +5400,56 @@
       <c r="A1" s="11"/>
     </row>
     <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="186" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="164" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="177" t="s">
+      <c r="C2" s="183" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="184" t="s">
+      <c r="E2" s="179" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="184" t="s">
+      <c r="G2" s="179" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="182" t="s">
+      <c r="H2" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="184" t="s">
+      <c r="I2" s="179" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="182" t="s">
+      <c r="J2" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="184" t="s">
+      <c r="K2" s="179" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="182" t="s">
+      <c r="L2" s="181" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="181"/>
-      <c r="B3" s="179"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="183"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="183"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="183"/>
+      <c r="A3" s="187"/>
+      <c r="B3" s="185"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="180"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180"/>
+      <c r="L3" s="182"/>
     </row>
     <row r="4" spans="1:14" ht="25.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
@@ -6094,7 +6094,7 @@
         <v>329</v>
       </c>
       <c r="D31" s="72" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E31" s="73"/>
       <c r="F31" s="72"/>
@@ -6118,6 +6118,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="H2:H3"/>
@@ -6125,11 +6130,6 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6140,7 +6140,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6267,11 +6267,11 @@
       <c r="A10" s="75" t="s">
         <v>330</v>
       </c>
-      <c r="B10" s="125" t="s">
-        <v>393</v>
-      </c>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
+      <c r="B10" s="127" t="s">
+        <v>388</v>
+      </c>
+      <c r="C10" s="127"/>
+      <c r="D10" s="127"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="58"/>
@@ -6286,10 +6286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6300,10 +6300,12 @@
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -6317,7 +6319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -6330,62 +6332,62 @@
       <c r="D3" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="37.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="37.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>157</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="39.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>159</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6394,7 +6396,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6413,48 +6415,48 @@
       <c r="A1" s="11"/>
     </row>
     <row r="2" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="95" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="94" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="92" t="s">
+      <c r="H2" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="92" t="s">
+      <c r="I2" s="94" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
+      <c r="A3" s="95"/>
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="92"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
     </row>
     <row r="4" spans="1:9" ht="124.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -6493,11 +6495,11 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
@@ -6588,7 +6590,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6610,20 +6612,20 @@
       <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="96" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="98"/>
-      <c r="B4" s="95"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="97"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="99"/>
-      <c r="B5" s="96"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="98"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="81" t="s">
@@ -6634,18 +6636,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="97"/>
+      <c r="B7" s="99"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="95"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="97"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
-      <c r="B9" s="96"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="98"/>
     </row>
     <row r="10" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -6656,36 +6658,36 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="97"/>
+      <c r="B11" s="99"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="98"/>
-      <c r="B12" s="95"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="97"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="99"/>
-      <c r="B13" s="96"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="98"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="97"/>
+      <c r="B15" s="99"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
-      <c r="B16" s="95"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="97"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="99"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="98"/>
     </row>
     <row r="18" spans="1:2" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -6720,11 +6722,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6736,403 +6739,407 @@
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+    <row r="3" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B3" s="55" t="s">
         <v>177</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C3" s="55" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D3" s="55" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:6" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="E3" s="93">
+        <v>45559</v>
+      </c>
+      <c r="F3" s="93"/>
+    </row>
+    <row r="4" spans="1:8" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B4" s="54" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>380</v>
-      </c>
-      <c r="D5" s="54" t="s">
+      <c r="C4" s="54" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="103" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="105" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="111" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="104"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="106"/>
+      <c r="F6" s="106"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="57">
+        <v>12415</v>
+      </c>
+      <c r="C7" s="57">
+        <v>8771</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="112" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="107" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="107" t="s">
+        <v>378</v>
+      </c>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="113"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+    </row>
+    <row r="10" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D10" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="B11" s="57">
+        <v>12415</v>
+      </c>
+      <c r="C11" s="57">
+        <v>8771</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="112" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="107" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="107" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="113"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="111" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="111" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="112" t="s">
+      <c r="E14" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="112" t="s">
+      <c r="F14" s="111" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="2" t="s">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="106"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B8" s="57">
-        <v>12415</v>
-      </c>
-      <c r="C8" s="57">
-        <v>8771</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+    </row>
+    <row r="16" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="82">
+        <v>5153</v>
+      </c>
+      <c r="C16" s="82">
+        <v>6820</v>
+      </c>
+      <c r="D16" s="82">
+        <v>1092</v>
+      </c>
+      <c r="E16" s="83" t="s">
+        <v>353</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="H16" s="58">
+        <f>C16+B16</f>
+        <v>11973</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="106" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" s="106" t="s">
-        <v>381</v>
-      </c>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
-    </row>
-    <row r="11" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="20" t="s">
+      <c r="B17" s="107" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" s="107" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="107" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="114"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="111" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C19" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D19" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F19" s="111" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>354</v>
-      </c>
-      <c r="B12" s="57">
-        <v>12415</v>
-      </c>
-      <c r="C12" s="57">
-        <v>8771</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="108" t="s">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="106"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+    </row>
+    <row r="21" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="B21" s="57">
+        <v>7262</v>
+      </c>
+      <c r="C21" s="57">
+        <v>1951</v>
+      </c>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="106" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="106" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-    </row>
-    <row r="14" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="110"/>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
-        <v>183</v>
-      </c>
-      <c r="B15" s="102" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="104" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="104" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="105"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-    </row>
-    <row r="17" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="B17" s="82">
-        <v>5153</v>
-      </c>
-      <c r="C17" s="82">
-        <v>6820</v>
-      </c>
-      <c r="D17" s="82">
-        <v>1092</v>
-      </c>
-      <c r="E17" s="83" t="s">
-        <v>353</v>
-      </c>
-      <c r="F17" s="23"/>
-      <c r="H17" s="58">
-        <f>C17+B17</f>
-        <v>11973</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="108" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="106" t="s">
+      <c r="B22" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="C18" s="106" t="s">
+      <c r="C22" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="D18" s="106" t="s">
-        <v>186</v>
-      </c>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109"/>
-      <c r="B19" s="107"/>
-      <c r="C19" s="107"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="104" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="102" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="104" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="104" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-    </row>
-    <row r="22" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="B22" s="57">
-        <v>7262</v>
-      </c>
-      <c r="C22" s="57">
-        <v>1951</v>
-      </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="108" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="106" t="s">
-        <v>185</v>
-      </c>
-      <c r="C23" s="106" t="s">
-        <v>185</v>
-      </c>
-      <c r="D23" s="106"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="109"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="101" t="s">
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="114"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="115" t="s">
         <v>351</v>
       </c>
-      <c r="C26" s="101"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C25" s="115"/>
+      <c r="D25" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>301</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E26" t="s">
         <v>302</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F26" t="s">
         <v>303</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="83" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7155,67 +7162,67 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="115" t="s">
+      <c r="E2" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
     </row>
     <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115"/>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115" t="s">
+      <c r="A3" s="116"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="115" t="s">
+      <c r="J3" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="115" t="s">
+      <c r="K3" s="116" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="116"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
+      <c r="A4" s="117"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
@@ -7360,17 +7367,17 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="90" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>304</v>
       </c>
-      <c r="C13" s="114" t="s">
+      <c r="C13" s="118" t="s">
         <v>355</v>
       </c>
-      <c r="D13" s="114"/>
+      <c r="D13" s="118"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
@@ -7379,6 +7386,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:K2"/>
@@ -7387,11 +7399,6 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7399,10 +7406,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7411,13 +7418,13 @@
     <col min="2" max="3" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
     </row>
-    <row r="3" spans="1:3" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>63</v>
       </c>
@@ -7428,8 +7435,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="100" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="122" t="s">
@@ -7439,29 +7446,29 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="99"/>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="101"/>
       <c r="B5" s="120"/>
       <c r="C5" s="120"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="121" t="s">
         <v>357</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="121" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="118"/>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="126"/>
       <c r="B7" s="123"/>
       <c r="C7" s="123"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="117" t="s">
+    <row r="8" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="125" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="124" t="s">
@@ -7471,58 +7478,61 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="101"/>
       <c r="B9" s="120"/>
       <c r="C9" s="120"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="100" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="119" t="s">
+      <c r="B10" s="121" t="s">
         <v>357</v>
       </c>
-      <c r="C10" s="119" t="s">
+      <c r="C10" s="121" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="101"/>
       <c r="B11" s="120"/>
       <c r="C11" s="120"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="100" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="121" t="s">
         <v>359</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="121" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="99"/>
+      <c r="D12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="101"/>
       <c r="B13" s="120"/>
       <c r="C13" s="120"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="100" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="C14" s="119"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="99"/>
+      <c r="C14" s="121"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="101"/>
       <c r="B15" s="120"/>
       <c r="C15" s="120"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>306</v>
       </c>
@@ -7530,8 +7540,23 @@
         <v>298</v>
       </c>
     </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>390</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B4:B5"/>
@@ -7540,16 +7565,6 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7559,8 +7574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7677,7 +7692,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="84" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B8" s="76" t="s">
         <v>361</v>
@@ -7712,16 +7727,18 @@
       <c r="A11" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="C11" s="125" t="s">
+      <c r="C11" s="127" t="s">
         <v>362</v>
       </c>
-      <c r="D11" s="125"/>
+      <c r="D11" s="127"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="18" t="s">
+        <v>391</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7737,7 +7754,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7757,35 +7774,35 @@
       <c r="A2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="116" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="116" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="116" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="115"/>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
+      <c r="A4" s="116"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
     </row>
     <row r="5" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>219</v>
@@ -7814,21 +7831,21 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="35.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="81" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="B7" s="85" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
       <c r="C7" s="85" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="D7" s="85" t="s">
-        <v>365</v>
+        <v>393</v>
       </c>
       <c r="E7" s="85" t="s">
-        <v>363</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
programacion de los indicadores
</commit_message>
<xml_diff>
--- a/Anotaciones.xlsx
+++ b/Anotaciones.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\progrmas_presupuestales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\progrmas_presupuestales\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AC5552-E322-4F78-AEF8-0337674D759A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="810" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="810" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato 1. Documentación de pol" sheetId="1" r:id="rId1"/>
@@ -33,22 +34,28 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Formato 5. Identificación y cua'!$A$1:$F$26</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Wilbert Suárez Solis</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -77,12 +84,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Wilbert Suárez Solis</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1562,7 +1569,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -2464,43 +2471,46 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2509,18 +2519,21 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2530,40 +2543,43 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2596,13 +2612,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2611,6 +2627,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
@@ -2620,15 +2651,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2641,83 +2663,68 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2757,7 +2764,7 @@
         <xdr:cNvPr id="8195" name="Text Box 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B088419-5395-49DB-ABCE-DCF627D04AAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B088419-5395-49DB-ABCE-DCF627D04AAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2837,7 +2844,7 @@
         <xdr:cNvPr id="8193" name="Text Box 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D505990-4389-48C5-81AE-2F28CAA46543}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D505990-4389-48C5-81AE-2F28CAA46543}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2917,7 +2924,7 @@
         <xdr:cNvPr id="8194" name="Text Box 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C4E20D9-3B0C-4E62-AC7D-D15BDAA741BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C4E20D9-3B0C-4E62-AC7D-D15BDAA741BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3278,7 +3285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -3409,7 +3416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3427,134 +3434,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="117" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="117" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
     </row>
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="132" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="130" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="135" t="s">
+      <c r="D3" s="128" t="s">
         <v>225</v>
       </c>
-      <c r="E3" s="135"/>
+      <c r="E3" s="128"/>
     </row>
     <row r="4" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="129"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
     </row>
     <row r="5" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="128" t="s">
+      <c r="B5" s="136" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="134" t="s">
         <v>259</v>
       </c>
-      <c r="D5" s="133" t="s">
+      <c r="D5" s="130" t="s">
         <v>227</v>
       </c>
-      <c r="E5" s="135" t="s">
+      <c r="E5" s="128" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="129"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="136"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="129"/>
     </row>
     <row r="7" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="136" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="134" t="s">
         <v>229</v>
       </c>
-      <c r="D7" s="133" t="s">
+      <c r="D7" s="130" t="s">
         <v>230</v>
       </c>
-      <c r="E7" s="135" t="s">
+      <c r="E7" s="128" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="129"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="136"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="129"/>
     </row>
     <row r="9" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="66"/>
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="136" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="134" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="133" t="s">
+      <c r="D9" s="130" t="s">
         <v>236</v>
       </c>
-      <c r="E9" s="135" t="s">
+      <c r="E9" s="128" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="136"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="135"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="129"/>
     </row>
     <row r="11" spans="1:5" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="66"/>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="136" t="s">
         <v>237</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="134" t="s">
         <v>238</v>
       </c>
-      <c r="D11" s="131" t="s">
+      <c r="D11" s="134" t="s">
         <v>239</v>
       </c>
-      <c r="E11" s="135" t="s">
+      <c r="E11" s="128" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="130"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="135"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="128"/>
     </row>
     <row r="13" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3701,6 +3708,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="B1:B2"/>
@@ -3714,17 +3732,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3732,7 +3739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3749,136 +3756,136 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="147" t="s">
+      <c r="A3" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="138" t="s">
+      <c r="B3" s="141" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="139"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="147" t="s">
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="138" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="147"/>
-      <c r="B4" s="141"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
-      <c r="G4" s="142"/>
-      <c r="H4" s="142"/>
-      <c r="I4" s="142"/>
-      <c r="J4" s="143"/>
-      <c r="K4" s="147"/>
+      <c r="A4" s="138"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="138"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="147"/>
-      <c r="B5" s="149" t="s">
+      <c r="A5" s="138"/>
+      <c r="B5" s="137" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="149" t="s">
+      <c r="C5" s="137" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="149" t="s">
+      <c r="D5" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="147" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="146"/>
-      <c r="K5" s="147"/>
+      <c r="F5" s="148"/>
+      <c r="G5" s="148"/>
+      <c r="H5" s="148"/>
+      <c r="I5" s="148"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="138"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="147"/>
-      <c r="B6" s="147"/>
-      <c r="C6" s="147"/>
-      <c r="D6" s="147"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="142"/>
-      <c r="J6" s="143"/>
-      <c r="K6" s="147"/>
+      <c r="A6" s="138"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="144"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="138"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="147"/>
-      <c r="B7" s="147"/>
-      <c r="C7" s="147"/>
-      <c r="D7" s="147"/>
-      <c r="E7" s="149" t="s">
+      <c r="A7" s="138"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="137" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="149" t="s">
+      <c r="F7" s="137" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="149" t="s">
+      <c r="G7" s="137" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="149" t="s">
+      <c r="H7" s="137" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="149" t="s">
+      <c r="I7" s="137" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="149" t="s">
+      <c r="J7" s="137" t="s">
         <v>94</v>
       </c>
-      <c r="K7" s="147"/>
+      <c r="K7" s="138"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="147"/>
-      <c r="B8" s="147"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="147"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="147"/>
-      <c r="H8" s="147"/>
-      <c r="I8" s="147"/>
-      <c r="J8" s="147"/>
-      <c r="K8" s="147"/>
+      <c r="A8" s="138"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="148"/>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
+      <c r="A9" s="139"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="139"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
@@ -3931,7 +3938,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="149" t="s">
+      <c r="A12" s="137" t="s">
         <v>96</v>
       </c>
       <c r="B12" s="121"/>
@@ -3946,17 +3953,17 @@
       <c r="K12" s="121"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="148"/>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
+      <c r="A13" s="139"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
     </row>
     <row r="14" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51" t="s">
@@ -4106,23 +4113,13 @@
       <c r="C19" s="64"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="115" t="s">
+      <c r="A21" s="103" t="s">
         <v>383</v>
       </c>
-      <c r="B21" s="115"/>
+      <c r="B21" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D5:D9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E7:E9"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:J4"/>
     <mergeCell ref="E5:J6"/>
@@ -4139,17 +4136,27 @@
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="K3:K9"/>
     <mergeCell ref="J7:J9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4163,22 +4170,22 @@
       <c r="A1" s="38"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="164"/>
-      <c r="B3" s="164"/>
-      <c r="C3" s="164"/>
+      <c r="A3" s="152"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
       <c r="E3" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="165" t="s">
+      <c r="A4" s="155" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="39" t="s">
@@ -4189,7 +4196,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="151"/>
+      <c r="A5" s="154"/>
       <c r="B5" s="26" t="s">
         <v>385</v>
       </c>
@@ -4201,34 +4208,34 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="156"/>
-      <c r="C6" s="157"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="158"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="150" t="s">
+      <c r="A7" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="163" t="s">
         <v>386</v>
       </c>
-      <c r="C7" s="159"/>
+      <c r="C7" s="164"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="151"/>
-      <c r="B8" s="160"/>
-      <c r="C8" s="161"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
     </row>
     <row r="9" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="163"/>
+      <c r="C9" s="151"/>
       <c r="E9" s="127" t="s">
         <v>368</v>
       </c>
@@ -4238,28 +4245,28 @@
       <c r="I9" s="127"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="152" t="s">
+      <c r="A10" s="160" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="153"/>
-      <c r="C10" s="154"/>
+      <c r="B10" s="161"/>
+      <c r="C10" s="162"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="162" t="s">
+      <c r="A11" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="B11" s="166"/>
-      <c r="C11" s="163"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="151"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="155" t="s">
+      <c r="A12" s="156" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="156"/>
-      <c r="C12" s="157"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="158"/>
     </row>
     <row r="13" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="150" t="s">
+      <c r="A13" s="153" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -4270,7 +4277,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="151"/>
+      <c r="A14" s="154"/>
       <c r="B14" s="40" t="s">
         <v>107</v>
       </c>
@@ -4279,7 +4286,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="150" t="s">
+      <c r="A15" s="153" t="s">
         <v>108</v>
       </c>
       <c r="B15" s="40" t="s">
@@ -4290,7 +4297,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="151"/>
+      <c r="A16" s="154"/>
       <c r="B16" s="40" t="s">
         <v>107</v>
       </c>
@@ -4299,7 +4306,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="150" t="s">
+      <c r="A17" s="153" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="40" t="s">
@@ -4308,14 +4315,14 @@
       <c r="C17" s="26"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="151"/>
+      <c r="A18" s="154"/>
       <c r="B18" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="153" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="40" t="s">
@@ -4324,18 +4331,18 @@
       <c r="C19" s="26"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="151"/>
+      <c r="A20" s="154"/>
       <c r="B20" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C20" s="26"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="152" t="s">
+      <c r="A21" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="153"/>
-      <c r="C21" s="154"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="162"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="41" t="s">
@@ -4360,11 +4367,11 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="157"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="158"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
@@ -4389,59 +4396,65 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="155" t="s">
+      <c r="A27" s="156" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="156"/>
-      <c r="C27" s="157"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="158"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="162" t="s">
+      <c r="B28" s="150" t="s">
         <v>265</v>
       </c>
-      <c r="C28" s="163"/>
+      <c r="C28" s="151"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="162" t="s">
+      <c r="B29" s="150" t="s">
         <v>266</v>
       </c>
-      <c r="C29" s="163"/>
+      <c r="C29" s="151"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="162" t="s">
+      <c r="B30" s="150" t="s">
         <v>267</v>
       </c>
-      <c r="C30" s="163"/>
+      <c r="C30" s="151"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="162" t="s">
+      <c r="B31" s="150" t="s">
         <v>268</v>
       </c>
-      <c r="C31" s="163"/>
+      <c r="C31" s="151"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="162" t="s">
+      <c r="B32" s="150" t="s">
         <v>269</v>
       </c>
-      <c r="C32" s="163"/>
+      <c r="C32" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="E9:I9"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="A2:C3"/>
@@ -4458,19 +4471,13 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4498,34 +4505,34 @@
       <c r="B2" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="117" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="116" t="s">
+      <c r="D2" s="117" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="116" t="s">
+      <c r="E2" s="117" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="116" t="s">
+      <c r="F2" s="117" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="116" t="s">
+      <c r="G2" s="117" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="116" t="s">
+      <c r="H2" s="117" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="168"/>
       <c r="B3" s="48"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
@@ -4770,7 +4777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4811,8 +4818,8 @@
     </row>
     <row r="4" spans="1:3" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="101"/>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122"/>
     </row>
     <row r="5" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
@@ -4838,8 +4845,8 @@
     </row>
     <row r="7" spans="1:3" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="101"/>
-      <c r="B7" s="120"/>
-      <c r="C7" s="120"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="102" t="s">
@@ -4854,8 +4861,8 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="101"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -4890,7 +4897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4912,166 +4919,166 @@
       <c r="A1" s="33"/>
     </row>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="106" t="s">
         <v>133</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="169" t="s">
+      <c r="C2" s="177" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="169" t="s">
+      <c r="E2" s="177" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="111" t="s">
+      <c r="F2" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="169" t="s">
+      <c r="G2" s="177" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="111" t="s">
+      <c r="H2" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="169" t="s">
+      <c r="I2" s="177" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="111" t="s">
+      <c r="J2" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="K2" s="169" t="s">
+      <c r="K2" s="177" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="111" t="s">
+      <c r="L2" s="106" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="106"/>
+      <c r="A3" s="107"/>
       <c r="B3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="169"/>
-      <c r="L3" s="111"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="106"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="169" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="171">
+      <c r="B4" s="174">
         <f>C4+E4+G4+I4+K4</f>
         <v>60019</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="174">
         <f>C6+C8</f>
         <v>11973</v>
       </c>
-      <c r="D4" s="172">
+      <c r="D4" s="175">
         <f>C4/$N$5</f>
         <v>0.56513735485698102</v>
       </c>
-      <c r="E4" s="171">
+      <c r="E4" s="174">
         <f>E6+E8</f>
         <v>11872</v>
       </c>
-      <c r="F4" s="172">
+      <c r="F4" s="175">
         <f>E4/$N$5</f>
         <v>0.56037005569715848</v>
       </c>
-      <c r="G4" s="171">
+      <c r="G4" s="174">
         <f>G6+G8</f>
         <v>12090</v>
       </c>
-      <c r="H4" s="172">
+      <c r="H4" s="175">
         <f>G4/$N$5</f>
         <v>0.57065986972529026</v>
       </c>
-      <c r="I4" s="171">
+      <c r="I4" s="174">
         <f>I6+I8</f>
         <v>11732</v>
       </c>
-      <c r="J4" s="172">
+      <c r="J4" s="175">
         <f>I4/$N$5</f>
         <v>0.55376191824789955</v>
       </c>
-      <c r="K4" s="171">
+      <c r="K4" s="174">
         <f>K6+K8</f>
         <v>12352</v>
       </c>
-      <c r="L4" s="172">
+      <c r="L4" s="175">
         <f>K4/$N$5</f>
         <v>0.5830265269517606</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="177"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="173"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="173"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="173"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="173"/>
+      <c r="A5" s="170"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="176"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="176"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="176"/>
       <c r="N5">
         <f>N6+N7</f>
         <v>21186</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="171">
+      <c r="B6" s="174">
         <f>C6+E6+G6+I6+K6</f>
         <v>26772</v>
       </c>
-      <c r="C6" s="171">
+      <c r="C6" s="174">
         <v>5153</v>
       </c>
-      <c r="D6" s="172">
+      <c r="D6" s="175">
         <f>C6/$N$6</f>
         <v>0.41506242448650826</v>
       </c>
-      <c r="E6" s="171">
+      <c r="E6" s="174">
         <v>5422</v>
       </c>
-      <c r="F6" s="172">
+      <c r="F6" s="175">
         <f>E6/$N$6</f>
         <v>0.43672976238421263</v>
       </c>
-      <c r="G6" s="171">
+      <c r="G6" s="174">
         <v>4890</v>
       </c>
-      <c r="H6" s="172">
+      <c r="H6" s="175">
         <f>G6/$N$6</f>
         <v>0.39387837293596456</v>
       </c>
-      <c r="I6" s="171">
+      <c r="I6" s="174">
         <v>5133</v>
       </c>
-      <c r="J6" s="172">
+      <c r="J6" s="175">
         <f>I6/$N$6</f>
         <v>0.4134514699959726</v>
       </c>
-      <c r="K6" s="171">
+      <c r="K6" s="174">
         <v>6174</v>
       </c>
-      <c r="L6" s="172">
+      <c r="L6" s="175">
         <f>K6/$N$6</f>
         <v>0.49730165122835279</v>
       </c>
@@ -5080,86 +5087,86 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="177"/>
-      <c r="B7" s="120"/>
-      <c r="C7" s="120"/>
-      <c r="D7" s="173"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="173"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="173"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="173"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="173"/>
+      <c r="A7" s="170"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="176"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="176"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="176"/>
       <c r="N7">
         <v>8771</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="169" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="171">
+      <c r="B8" s="174">
         <f>C8+E8+G8+I8+K8</f>
         <v>33247</v>
       </c>
-      <c r="C8" s="171">
+      <c r="C8" s="174">
         <v>6820</v>
       </c>
-      <c r="D8" s="172">
+      <c r="D8" s="175">
         <f>C8/$N$7</f>
         <v>0.77756242161669142</v>
       </c>
-      <c r="E8" s="171">
+      <c r="E8" s="174">
         <v>6450</v>
       </c>
-      <c r="F8" s="172">
+      <c r="F8" s="175">
         <f>E8/$N$7</f>
         <v>0.73537795006270668</v>
       </c>
-      <c r="G8" s="171">
+      <c r="G8" s="174">
         <v>7200</v>
       </c>
-      <c r="H8" s="172">
+      <c r="H8" s="175">
         <f>G8/$N$7</f>
         <v>0.82088701402348652</v>
       </c>
-      <c r="I8" s="171">
+      <c r="I8" s="174">
         <v>6599</v>
       </c>
-      <c r="J8" s="172">
+      <c r="J8" s="175">
         <f>I8/$N$7</f>
         <v>0.75236575076958156</v>
       </c>
-      <c r="K8" s="171">
+      <c r="K8" s="174">
         <v>6178</v>
       </c>
-      <c r="L8" s="172">
+      <c r="L8" s="175">
         <f>K8/$N$7</f>
         <v>0.70436666286626382</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="177"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="173"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="173"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="173"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="173"/>
+      <c r="A9" s="170"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="176"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="176"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="176"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="176"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="169" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="121"/>
-      <c r="C10" s="171">
+      <c r="C10" s="174">
         <v>1092</v>
       </c>
       <c r="D10" s="121"/>
@@ -5173,24 +5180,24 @@
       <c r="L10" s="121"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="177"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="122"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="169" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="174" t="s">
+      <c r="B12" s="172" t="s">
         <v>387</v>
       </c>
       <c r="C12" s="121"/>
@@ -5205,24 +5212,24 @@
       <c r="L12" s="121"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="177"/>
-      <c r="B13" s="175"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
+      <c r="A13" s="170"/>
+      <c r="B13" s="173"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="122"/>
     </row>
     <row r="14" spans="1:14" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="176" t="s">
+      <c r="A14" s="169" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="174" t="s">
+      <c r="B14" s="172" t="s">
         <v>163</v>
       </c>
       <c r="C14" s="121"/>
@@ -5237,32 +5244,32 @@
       <c r="L14" s="121"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="177"/>
-      <c r="B15" s="175"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
+      <c r="A15" s="170"/>
+      <c r="B15" s="173"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="122"/>
+      <c r="H15" s="122"/>
+      <c r="I15" s="122"/>
+      <c r="J15" s="122"/>
+      <c r="K15" s="122"/>
+      <c r="L15" s="122"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="178" t="s">
+      <c r="A16" s="171" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="178"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
+      <c r="B16" s="171"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="178" t="s">
+      <c r="A17" s="171" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="178"/>
+      <c r="B17" s="171"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
     </row>
@@ -5283,11 +5290,70 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
@@ -5304,70 +5370,11 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5375,7 +5382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5400,56 +5407,56 @@
       <c r="A1" s="11"/>
     </row>
     <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="182" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="152" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="183" t="s">
+      <c r="C2" s="179" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="181" t="s">
+      <c r="D2" s="184" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="179" t="s">
+      <c r="E2" s="186" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="181" t="s">
+      <c r="F2" s="184" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="179" t="s">
+      <c r="G2" s="186" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="181" t="s">
+      <c r="H2" s="184" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="179" t="s">
+      <c r="I2" s="186" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="181" t="s">
+      <c r="J2" s="184" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="179" t="s">
+      <c r="K2" s="186" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="181" t="s">
+      <c r="L2" s="184" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="187"/>
-      <c r="B3" s="185"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="180"/>
-      <c r="L3" s="182"/>
+      <c r="A3" s="183"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="185"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="185"/>
     </row>
     <row r="4" spans="1:14" ht="25.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
@@ -6118,11 +6125,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="H2:H3"/>
@@ -6130,13 +6132,18 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6285,7 +6292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
@@ -6392,7 +6399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6586,7 +6593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6721,7 +6728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6802,19 +6809,19 @@
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="114" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="105" t="s">
+      <c r="F5" s="114" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6822,13 +6829,13 @@
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="106"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="107"/>
       <c r="D6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
@@ -6845,26 +6852,26 @@
       <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="108" t="s">
         <v>180</v>
       </c>
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="108" t="s">
         <v>378</v>
       </c>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="113"/>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
+      <c r="A9" s="112"/>
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="115"/>
     </row>
     <row r="10" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -6901,56 +6908,56 @@
       <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="112" t="s">
+      <c r="A12" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="108" t="s">
         <v>180</v>
       </c>
-      <c r="C12" s="107" t="s">
+      <c r="C12" s="108" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
-      <c r="B13" s="108"/>
-      <c r="C13" s="108"/>
+      <c r="A13" s="112"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="109"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="108"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="111" t="s">
+      <c r="C14" s="106" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="111" t="s">
+      <c r="E14" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="111" t="s">
+      <c r="F14" s="106" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="106"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="106"/>
+      <c r="A15" s="107"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="107"/>
       <c r="D15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
     </row>
     <row r="16" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
@@ -6975,23 +6982,23 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="112" t="s">
+      <c r="A17" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="108" t="s">
         <v>185</v>
       </c>
-      <c r="C17" s="107" t="s">
+      <c r="C17" s="108" t="s">
         <v>185</v>
       </c>
-      <c r="D17" s="107" t="s">
+      <c r="D17" s="108" t="s">
         <v>186</v>
       </c>
-      <c r="E17" s="107"/>
-      <c r="F17" s="107"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="114"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="109"/>
       <c r="C18" s="109"/>
       <c r="D18" s="109"/>
@@ -6999,34 +7006,34 @@
       <c r="F18" s="109"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="111" t="s">
+      <c r="A19" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="111" t="s">
+      <c r="C19" s="106" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="111" t="s">
+      <c r="E19" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="111" t="s">
+      <c r="F19" s="106" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="106"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="106"/>
+      <c r="A20" s="107"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="107"/>
       <c r="D20" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
     </row>
     <row r="21" spans="1:6" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
@@ -7043,21 +7050,21 @@
       <c r="F21" s="55"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="112" t="s">
+      <c r="A22" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="108" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="107" t="s">
+      <c r="C22" s="108" t="s">
         <v>185</v>
       </c>
-      <c r="D22" s="107"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="107"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="108"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="114"/>
+      <c r="A23" s="111"/>
       <c r="B23" s="109"/>
       <c r="C23" s="109"/>
       <c r="D23" s="109"/>
@@ -7065,10 +7072,10 @@
       <c r="F23" s="109"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="115" t="s">
+      <c r="B25" s="103" t="s">
         <v>351</v>
       </c>
-      <c r="C25" s="115"/>
+      <c r="C25" s="103"/>
       <c r="D25" t="s">
         <v>389</v>
       </c>
@@ -7086,31 +7093,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
@@ -7125,6 +7107,31 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" orientation="landscape" r:id="rId1"/>
@@ -7132,13 +7139,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -7162,67 +7169,67 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="116" t="s">
+      <c r="D2" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="116" t="s">
+      <c r="E2" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="116" t="s">
+      <c r="F2" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
     </row>
     <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116"/>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116" t="s">
+      <c r="A3" s="117"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="116" t="s">
+      <c r="G3" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="116" t="s">
+      <c r="H3" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="116" t="s">
+      <c r="I3" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="116" t="s">
+      <c r="J3" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="116" t="s">
+      <c r="K3" s="117" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
@@ -7374,10 +7381,10 @@
       <c r="B13" t="s">
         <v>304</v>
       </c>
-      <c r="C13" s="118" t="s">
+      <c r="C13" s="116" t="s">
         <v>355</v>
       </c>
-      <c r="D13" s="118"/>
+      <c r="D13" s="116"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
@@ -7386,11 +7393,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B2:B4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:K2"/>
@@ -7399,13 +7401,18 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7439,17 +7446,17 @@
       <c r="A4" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="124" t="s">
         <v>356</v>
       </c>
-      <c r="C4" s="122" t="s">
+      <c r="C4" s="124" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="101"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="102" t="s">
@@ -7463,25 +7470,25 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="126"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
+      <c r="A7" s="120"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="125" t="s">
+      <c r="A8" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="124" t="s">
+      <c r="B8" s="126" t="s">
         <v>358</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="126" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="101"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="102" t="s">
@@ -7496,8 +7503,8 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="101"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="122"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="102" t="s">
@@ -7515,22 +7522,22 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="101"/>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="122"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="123" t="s">
         <v>360</v>
       </c>
       <c r="C14" s="121"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="101"/>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="122"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -7547,16 +7554,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B4:B5"/>
@@ -7565,13 +7562,23 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -7750,7 +7757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7774,28 +7781,28 @@
       <c r="A2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="117" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="117" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="116" t="s">
+      <c r="E3" s="117" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="116"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
+      <c r="A4" s="117"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
     </row>
     <row r="5" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">

</xml_diff>